<commit_message>
Update Glosario y Reseñas  Pueblos GT.xlsx
</commit_message>
<xml_diff>
--- a/Glosario y Reseñas  Pueblos GT.xlsx
+++ b/Glosario y Reseñas  Pueblos GT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo Arancibia\Dropbox\Diseño DATA's (1)\DATA-PUEBLOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paula\DATA INTELLIGENCE Dropbox\Diseño DATA's\DATA-PUEBLOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD9B744-64DA-4116-B77E-B114BC8BF92B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AC2331-F746-4B01-A9B2-085C5865942D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A42F21A4-5D28-4FF8-89B3-B9A631EB2D69}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A42F21A4-5D28-4FF8-89B3-B9A631EB2D69}"/>
   </bookViews>
   <sheets>
     <sheet name="Glosario Data Pueblos GT" sheetId="28" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="181">
   <si>
     <t xml:space="preserve">GLOSARIO DATA PUEBLOS </t>
   </si>
@@ -974,8 +974,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{89E5B61D-1371-4FEF-88B9-BDCFD5B4CFE7}" name="Glosario_general_CL_GT" displayName="Glosario_general_CL_GT" ref="A1:C8" totalsRowShown="0">
-  <autoFilter ref="A1:C8" xr:uid="{B9CD52D0-84A3-48BA-8208-56A6B125E7A4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{89E5B61D-1371-4FEF-88B9-BDCFD5B4CFE7}" name="Glosario_general_CL_GT" displayName="Glosario_general_CL_GT" ref="A1:C9" totalsRowShown="0">
+  <autoFilter ref="A1:C9" xr:uid="{B9CD52D0-84A3-48BA-8208-56A6B125E7A4}"/>
   <tableColumns count="3">
     <tableColumn id="3" xr3:uid="{47829CA8-0F6A-4244-8BF8-BBB5D59C6D87}" name="Código"/>
     <tableColumn id="1" xr3:uid="{8B8DA6DF-08A2-42F9-A052-6A16A843C3F4}" name="Concepto"/>
@@ -1311,7 +1311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F3EE3A-1C26-4EA7-A289-72E3B06B5B99}">
   <dimension ref="A2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
@@ -1840,10 +1840,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F26D00-5F21-4445-BCDB-408F9A4965AD}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,6 +1938,17 @@
       </c>
       <c r="C8" s="8" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2289,7 +2300,7 @@
   <dimension ref="A2:B10"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>